<commit_message>
Iteration 1 - Updated with 17 stored procs
</commit_message>
<xml_diff>
--- a/AgileDevelopmentProcess.xlsx
+++ b/AgileDevelopmentProcess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Angular\Market_Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9556D85E-D19A-4871-AFA3-84B141784F09}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897B548E-CB70-40F8-9190-C00AE39B6586}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="945" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="2" xr2:uid="{9DCCD3A2-661B-4281-B578-9CF138C47E9D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{9DCCD3A2-661B-4281-B578-9CF138C47E9D}"/>
   </bookViews>
   <sheets>
     <sheet name="StandUpMeetings" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="111">
   <si>
     <t>PBI_ID</t>
   </si>
@@ -329,6 +329,100 @@
   </si>
   <si>
     <t>Customer table stored procedures</t>
+  </si>
+  <si>
+    <t>Future Changes</t>
+  </si>
+  <si>
+    <t>Product discount</t>
+  </si>
+  <si>
+    <t>As a Product Owner, I want to define the discount on products</t>
+  </si>
+  <si>
+    <t>Generate Barcode</t>
+  </si>
+  <si>
+    <t>As a Product Owner, I want to define the Barcode for each product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP1 =&gt;
+	Name: GetShopByContactNumber
+	Input: Contact_Number
+	Output: should return =&gt; Shop_No, Shop_Name, Shop_Address Contact_Number1, Contact_Number2 
+</t>
+  </si>
+  <si>
+    <t>Product Count</t>
+  </si>
+  <si>
+    <t>As a Product Owner, I want to keep track of how many product available in a shop?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP1 =&gt;
+	Name: GetProductByProductName
+	Input: Product_Name
+	Output: should return =&gt; Product_Name, Product_Type, Product_Tax, Product_Price 
+</t>
+  </si>
+  <si>
+    <t>As a Product Owner, I want to import shop and product details using csv, txt or excel files</t>
+  </si>
+  <si>
+    <t>Import Shop and Product details using data files</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence ordering</t>
+  </si>
+  <si>
+    <t>As a Product Owner, I want to accept the online orders using Artificial Intelligence(Speech decoding)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP2 =&gt;
+	Name: GetAllProductByProductPriceRange
+	Input: Min_Price, Max_Price
+	Output: should return =&gt; Product_Name, Product_Type, Product_Tax, Product_Price 
+</t>
+  </si>
+  <si>
+    <t>SP4 =&gt; 
+	Name: GetAllShopAndProductCount
+	Input: No Input
+	Output: should return =&gt; Shop_No, ShopName, Product_Count
+Hint: Use Having and Order by clause</t>
+  </si>
+  <si>
+    <t>SP1 =&gt; 
+	Name: GetOrderDetails
+	Input: Order_Id
+	Output: should return =&gt; 
+Shop Details: Shop Name, Shop_Address, Contact_Number1
+Product Details: Product_Name, Product_Type, Product_Price
+Billing Details: Billing_Amount, Tax_Amount, Total_Amount
+Payment Details: Payment_Type, Pay_Status
+Customer Details: First_Name, Last_Name, Contact_Number
+Hint: Use Having and Order by clause</t>
+  </si>
+  <si>
+    <t>SP1 =&gt; 
+	Name: GetPaymentByCustomerName
+	Input: Customer_Name
+	Output: should return =&gt; First_Name, Last_Name, Contact_Number, Payment_Type, Pay_Status
+Hint: Use Having and Order by clause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP1 =&gt; 
+	Name: GetCustomerByProductName
+	Input: Product_Name
+	Output: should return =&gt; First_Name, Last_Name, Contact_Number, Product_Name, Product_Price
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP1 =&gt; 
+	Name: GetPaymentByCustomerName
+	Input: Customer_Name
+	Output: should return =&gt; First_Name, Last_Name, Contact_Number, Payment_Type, Pay_Status
+</t>
   </si>
 </sst>
 </file>
@@ -352,7 +446,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,6 +456,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -542,23 +642,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -568,53 +684,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,26 +1052,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="9">
+      <c r="A1" s="18">
         <v>43535</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="D1" s="9">
+      <c r="B1" s="19"/>
+      <c r="D1" s="18">
         <v>43536</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="G1" s="9">
+      <c r="E1" s="19"/>
+      <c r="G1" s="18">
         <v>43537</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="J1" s="9">
+      <c r="H1" s="19"/>
+      <c r="J1" s="18">
         <v>43538</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="M1" s="9">
+      <c r="K1" s="19"/>
+      <c r="M1" s="18">
         <v>43539</v>
       </c>
-      <c r="N1" s="10"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1058,26 +1159,26 @@
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="18">
         <v>43535</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="D6" s="9">
+      <c r="B6" s="19"/>
+      <c r="D6" s="18">
         <v>43536</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="G6" s="9">
+      <c r="E6" s="19"/>
+      <c r="G6" s="18">
         <v>43537</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="J6" s="9">
+      <c r="H6" s="19"/>
+      <c r="J6" s="18">
         <v>43538</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="M6" s="9">
+      <c r="K6" s="19"/>
+      <c r="M6" s="18">
         <v>43539</v>
       </c>
-      <c r="N6" s="10"/>
+      <c r="N6" s="19"/>
     </row>
     <row r="7" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1153,26 +1254,26 @@
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="18">
         <v>43535</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="D11" s="9">
+      <c r="B11" s="19"/>
+      <c r="D11" s="18">
         <v>43536</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="G11" s="9">
+      <c r="E11" s="19"/>
+      <c r="G11" s="18">
         <v>43537</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="J11" s="9">
+      <c r="H11" s="19"/>
+      <c r="J11" s="18">
         <v>43538</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="M11" s="9">
+      <c r="K11" s="19"/>
+      <c r="M11" s="18">
         <v>43539</v>
       </c>
-      <c r="N11" s="10"/>
+      <c r="N11" s="19"/>
     </row>
     <row r="12" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1248,26 +1349,26 @@
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="18">
         <v>43535</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="D16" s="9">
+      <c r="B16" s="19"/>
+      <c r="D16" s="18">
         <v>43536</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="G16" s="9">
+      <c r="E16" s="19"/>
+      <c r="G16" s="18">
         <v>43537</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="J16" s="9">
+      <c r="H16" s="19"/>
+      <c r="J16" s="18">
         <v>43538</v>
       </c>
-      <c r="K16" s="10"/>
-      <c r="M16" s="9">
+      <c r="K16" s="19"/>
+      <c r="M16" s="18">
         <v>43539</v>
       </c>
-      <c r="N16" s="10"/>
+      <c r="N16" s="19"/>
     </row>
     <row r="17" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -1343,26 +1444,26 @@
     </row>
     <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="18">
         <v>43535</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="D21" s="9">
+      <c r="B21" s="19"/>
+      <c r="D21" s="18">
         <v>43536</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="G21" s="9">
+      <c r="E21" s="19"/>
+      <c r="G21" s="18">
         <v>43537</v>
       </c>
-      <c r="H21" s="10"/>
-      <c r="J21" s="9">
+      <c r="H21" s="19"/>
+      <c r="J21" s="18">
         <v>43538</v>
       </c>
-      <c r="K21" s="10"/>
-      <c r="M21" s="9">
+      <c r="K21" s="19"/>
+      <c r="M21" s="18">
         <v>43539</v>
       </c>
-      <c r="N21" s="10"/>
+      <c r="N21" s="19"/>
     </row>
     <row r="22" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1438,26 +1539,26 @@
     </row>
     <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="A26" s="18">
         <v>43535</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="D26" s="9">
+      <c r="B26" s="19"/>
+      <c r="D26" s="18">
         <v>43536</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="G26" s="9">
+      <c r="E26" s="19"/>
+      <c r="G26" s="18">
         <v>43537</v>
       </c>
-      <c r="H26" s="10"/>
-      <c r="J26" s="9">
+      <c r="H26" s="19"/>
+      <c r="J26" s="18">
         <v>43538</v>
       </c>
-      <c r="K26" s="10"/>
-      <c r="M26" s="9">
+      <c r="K26" s="19"/>
+      <c r="M26" s="18">
         <v>43539</v>
       </c>
-      <c r="N26" s="10"/>
+      <c r="N26" s="19"/>
     </row>
     <row r="27" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
@@ -1533,36 +1634,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="M11:N11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="M26:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1570,26 +1671,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E8FB7F-543E-476A-957C-6771AF74EF60}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.140625" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1597,10 +1698,10 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1608,10 +1709,10 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1619,10 +1720,10 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1630,21 +1731,21 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1652,10 +1753,10 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1663,14 +1764,112 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="9" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>8</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>9</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>10</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>11</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>12</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>13</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:C11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1678,481 +1877,519 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356D0133-11B9-4AEC-A417-E1C8307FD7E9}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="21"/>
-    <col min="2" max="2" width="10" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="12"/>
+    <col min="2" max="2" width="10" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" style="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="15" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="11">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="32">
+      <c r="A3" s="26"/>
+      <c r="B3" s="11">
         <v>2</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="32">
+      <c r="A4" s="26"/>
+      <c r="B4" s="11">
         <v>3</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="32">
+      <c r="A5" s="26"/>
+      <c r="B5" s="11">
         <v>4</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="32">
+      <c r="A6" s="26"/>
+      <c r="B6" s="11">
         <v>5</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="32">
+      <c r="A7" s="26"/>
+      <c r="B7" s="11">
         <v>6</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="32">
+      <c r="A8" s="26"/>
+      <c r="B8" s="11">
         <v>7</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="14"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="20">
         <v>2</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="11">
         <v>1</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="32">
+      <c r="A11" s="21"/>
+      <c r="B11" s="11">
         <v>2</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="9" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="32">
+      <c r="A12" s="21"/>
+      <c r="B12" s="11">
         <v>3</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="9" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="32">
+      <c r="A13" s="21"/>
+      <c r="B13" s="11">
         <v>4</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="32">
+      <c r="A14" s="21"/>
+      <c r="B14" s="11">
         <v>5</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="32">
+      <c r="A15" s="21"/>
+      <c r="B15" s="11">
         <v>6</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="32">
+      <c r="A16" s="21"/>
+      <c r="B16" s="11">
         <v>7</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="9" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="32">
+      <c r="A17" s="21"/>
+      <c r="B17" s="11">
         <v>8</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="32">
+      <c r="A18" s="21"/>
+      <c r="B18" s="11">
         <v>9</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="32">
+      <c r="A19" s="22"/>
+      <c r="B19" s="11">
         <v>10</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
+      <c r="A20" s="20">
         <v>3</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="11">
         <v>1</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="32">
+      <c r="A21" s="21"/>
+      <c r="B21" s="11">
         <v>2</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="32">
+      <c r="A22" s="21"/>
+      <c r="B22" s="11">
         <v>3</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="32">
+      <c r="A23" s="21"/>
+      <c r="B23" s="11">
         <v>4</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="32">
+      <c r="A24" s="21"/>
+      <c r="B24" s="11">
         <v>5</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="32">
+      <c r="A25" s="21"/>
+      <c r="B25" s="11">
         <v>6</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="32">
+      <c r="A26" s="21"/>
+      <c r="B26" s="11">
         <v>7</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="32">
+      <c r="A27" s="21"/>
+      <c r="B27" s="11">
         <v>8</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="32">
+      <c r="A28" s="21"/>
+      <c r="B28" s="11">
         <v>9</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="9" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="32">
+      <c r="A29" s="21"/>
+      <c r="B29" s="11">
         <v>10</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="9" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="16">
+      <c r="A30" s="21"/>
+      <c r="B30" s="20">
         <v>11</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="14" t="s">
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="14" t="s">
+    <row r="32" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="14" t="s">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="14" t="s">
+      <c r="A34" s="21"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-      <c r="B35" s="32">
+    <row r="35" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="11">
         <v>12</v>
       </c>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D35" s="14"/>
-    </row>
-    <row r="36" spans="1:4" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
-      <c r="B36" s="32">
+      <c r="D35" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+      <c r="B36" s="20">
         <v>13</v>
       </c>
-      <c r="C36" s="33" t="s">
+      <c r="C36" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="14"/>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="32">
-        <v>14</v>
-      </c>
-      <c r="C37" s="34" t="s">
+      <c r="D36" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+      <c r="B40" s="11">
+        <v>14</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="13"/>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="32">
+      <c r="D40" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+      <c r="B41" s="11">
         <v>15</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C41" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="13"/>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="32">
-        <v>16</v>
-      </c>
-      <c r="C39" s="34" t="s">
+      <c r="D41" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+      <c r="B42" s="11">
+        <v>16</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="13"/>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="32">
-        <v>17</v>
-      </c>
-      <c r="C40" s="34" t="s">
+      <c r="D42" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A43" s="22"/>
+      <c r="B43" s="11">
+        <v>17</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D40" s="13"/>
+      <c r="D43" s="9" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A20:A43"/>
     <mergeCell ref="B30:B34"/>
     <mergeCell ref="C30:C34"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A10:A19"/>
-    <mergeCell ref="A20:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>